<commit_message>
Added trade balance of chile and argentina
</commit_message>
<xml_diff>
--- a/code/data/trade balance.xlsx
+++ b/code/data/trade balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\Github\GitHub\Advanced-Time-Series-Analysis-Article-Replication\code\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7EFF0C-5A8A-4077-9202-36CED07D3769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260F56D9-3A0A-4C9C-B948-2C5CC925EAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -184,7 +184,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -470,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="95" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -635,8 +635,12 @@
       <c r="F2" s="2">
         <v>0.11074347000661365</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G2" s="1">
+        <v>1.3692063491878286E-3</v>
+      </c>
+      <c r="H2" s="1">
+        <v>6.8412708182877757E-2</v>
+      </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -683,8 +687,12 @@
       <c r="F3" s="2">
         <v>6.4501649348724082E-3</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="1">
+        <v>4.308324331204841E-3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>6.4995210458394029E-3</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -731,8 +739,12 @@
       <c r="F4" s="2">
         <v>4.1271257579685644E-3</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="1">
+        <v>1.976924958845481E-3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>2.1619299784110977E-3</v>
+      </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -779,8 +791,12 @@
       <c r="F5" s="2">
         <v>8.4673661972791067E-3</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1">
+        <v>3.9771966452856146E-3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>9.2630940159217703E-3</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -827,8 +843,12 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="1">
+        <v>5.5595606294933271E-3</v>
+      </c>
+      <c r="H6" s="1">
+        <v>7.8608062076568883E-2</v>
+      </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -878,7 +898,9 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>1.9577022433118794E-2</v>
+      </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -925,7 +947,9 @@
       <c r="F8" s="1">
         <v>2.7745953263503077E-2</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>2.2183296827899711E-3</v>
+      </c>
       <c r="H8" s="1">
         <v>0</v>
       </c>
@@ -975,8 +999,12 @@
       <c r="F9" s="1">
         <v>0.1167756468775026</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="1">
+        <v>5.0404356826799453E-2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.146760205514747</v>
+      </c>
       <c r="I9" s="1">
         <v>0</v>
       </c>
@@ -1025,8 +1053,12 @@
       <c r="F10" s="1">
         <v>4.3291734453536094E-3</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="G10" s="1">
+        <v>1.6913107502923154E-3</v>
+      </c>
+      <c r="H10" s="1">
+        <v>5.4608938159211376E-3</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1">
         <v>0</v>
@@ -1075,8 +1107,12 @@
       <c r="F11" s="1">
         <v>3.1083754212527626E-2</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1">
+        <v>1.0782525397039697E-2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>3.2028659801896335E-2</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1">
@@ -1125,8 +1161,12 @@
       <c r="F12" s="1">
         <v>7.443826884837447E-2</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="G12" s="1">
+        <v>1.903889017852782E-2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>4.1999466319479518E-2</v>
+      </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -1175,8 +1215,12 @@
       <c r="F13" s="1">
         <v>1.5521850825187958E-2</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1">
+        <v>4.4685195258601122E-3</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.3166665929954888E-2</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
@@ -1225,8 +1269,12 @@
       <c r="F14" s="1">
         <v>7.7852476681984344E-3</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1">
+        <v>2.8052913600327329E-3</v>
+      </c>
+      <c r="H14" s="1">
+        <v>4.8277764365049422E-3</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
@@ -1275,8 +1323,12 @@
       <c r="F15" s="1">
         <v>4.0604041969260998E-2</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="G15" s="1">
+        <v>9.3185386423126522E-3</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3.3638334016656328E-2</v>
+      </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
@@ -1325,8 +1377,12 @@
       <c r="F16" s="1">
         <v>5.3209511514685885E-2</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="G16" s="1">
+        <v>3.610110338906148E-2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0.10218520323376894</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
@@ -1375,8 +1431,12 @@
       <c r="F17" s="1">
         <v>2.7612074630736106E-2</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="G17" s="1">
+        <v>1.1864402104013429E-2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>5.0965214515899852E-2</v>
+      </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1425,8 +1485,12 @@
       <c r="F18" s="1">
         <v>8.8869361242340725E-3</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="G18" s="1">
+        <v>3.8582892097878685E-3</v>
+      </c>
+      <c r="H18" s="1">
+        <v>4.258467472522235E-3</v>
+      </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1475,8 +1539,12 @@
       <c r="F19" s="1">
         <v>2.7259918008150728E-2</v>
       </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
+      <c r="G19" s="1">
+        <v>2.6318240770361975E-2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.442203013679155E-2</v>
+      </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
@@ -1525,8 +1593,12 @@
       <c r="F20" s="1">
         <v>4.5223300777215168E-2</v>
       </c>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="G20" s="1">
+        <v>6.2994532718689275E-3</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2.5402891772702517E-2</v>
+      </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
@@ -1575,8 +1647,12 @@
       <c r="F21" s="1">
         <v>6.7006619356575498E-4</v>
       </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="G21" s="1">
+        <v>1.1133878815264115E-3</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1.4416019419556114E-3</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
@@ -1625,8 +1701,12 @@
       <c r="F22" s="1">
         <v>4.6736826125447408E-3</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="1">
+        <v>6.7346391872101976E-3</v>
+      </c>
+      <c r="H22" s="1">
+        <v>2.0102818388245359E-3</v>
+      </c>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
@@ -1675,8 +1755,12 @@
       <c r="F23" s="1">
         <v>9.2739670718785562E-3</v>
       </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="G23" s="1">
+        <v>2.2818142329625525E-3</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2.4399845245343967E-2</v>
+      </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
@@ -1725,8 +1809,12 @@
       <c r="F24" s="1">
         <v>3.1224961076641586E-3</v>
       </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="G24" s="1">
+        <v>1.9165744914559891E-3</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2.3215991626261566E-3</v>
+      </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1775,8 +1863,12 @@
       <c r="F25" s="1">
         <v>1.9519941393771775E-2</v>
       </c>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="G25" s="1">
+        <v>3.0565296254589265E-3</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2.1129762353883116E-3</v>
+      </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
@@ -1825,8 +1917,12 @@
       <c r="F26" s="1">
         <v>9.2972626076749214E-3</v>
       </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
+      <c r="G26" s="1">
+        <v>2.753525593717999E-3</v>
+      </c>
+      <c r="H26" s="1">
+        <v>2.5340394344447285E-3</v>
+      </c>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
@@ -1875,8 +1971,12 @@
       <c r="F27" s="1">
         <v>7.4527762181633367E-3</v>
       </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
+      <c r="G27" s="1">
+        <v>1.383892948543576E-3</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3.3237048534007899E-3</v>
+      </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
@@ -1925,8 +2025,12 @@
       <c r="F28" s="1">
         <v>2.2817728831469132E-2</v>
       </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
+      <c r="G28" s="1">
+        <v>3.1704982610042567E-3</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2.7100514716600528E-2</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -1975,8 +2079,12 @@
       <c r="F29" s="1">
         <v>9.1253020917953804E-3</v>
       </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
+      <c r="G29" s="1">
+        <v>3.1597042241112466E-3</v>
+      </c>
+      <c r="H29" s="1">
+        <v>8.7208044984381488E-3</v>
+      </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -2025,8 +2133,12 @@
       <c r="F30" s="1">
         <v>1.4204065697058654E-2</v>
       </c>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="1">
+        <v>4.6269941909028167E-3</v>
+      </c>
+      <c r="H30" s="1">
+        <v>6.9768499414119981E-3</v>
+      </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -2075,8 +2187,12 @@
       <c r="F31" s="1">
         <v>8.7095143334020731E-3</v>
       </c>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="G31" s="1">
+        <v>3.5952886843627946E-3</v>
+      </c>
+      <c r="H31" s="1">
+        <v>6.4010524310865093E-3</v>
+      </c>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -2125,8 +2241,12 @@
       <c r="F32" s="1">
         <v>4.8931218014147048E-3</v>
       </c>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="G32" s="1">
+        <v>1.653873720662527E-3</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.9542577097694412E-3</v>
+      </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -2175,8 +2295,12 @@
       <c r="F33" s="1">
         <v>2.7167574209157386E-2</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="G33" s="1">
+        <v>2.5105076174573002E-2</v>
+      </c>
+      <c r="H33" s="1">
+        <v>2.7240802090799088E-2</v>
+      </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -2225,8 +2349,12 @@
       <c r="F34" s="1">
         <v>0.23002085221016386</v>
       </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="G34" s="1">
+        <v>0.73708773676074224</v>
+      </c>
+      <c r="H34" s="1">
+        <v>0.2018235232003272</v>
+      </c>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>

</xml_diff>